<commit_message>
add api update email for student controller
</commit_message>
<xml_diff>
--- a/import-demo-student-list.xlsx
+++ b/import-demo-student-list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Boku no\InternshipProject\student-fita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E99D7B8-6EB3-4423-8DBF-178E454CE27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B723DC3-AA11-40FC-9A32-FBBE16D79A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0A5968B0-B636-4779-A398-BA415D297B06}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Hà Nội</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Số điện thoại</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>66</t>
   </si>
   <si>
@@ -102,12 +99,6 @@
     <t>0383817445</t>
   </si>
   <si>
-    <t>ntb@gmail.com</t>
-  </si>
-  <si>
-    <t>nlc@gmail.com</t>
-  </si>
-  <si>
     <t>Ngành</t>
   </si>
   <si>
@@ -139,9 +130,6 @@
   </si>
   <si>
     <t>Dương</t>
-  </si>
-  <si>
-    <t>ntd@gmail.com</t>
   </si>
   <si>
     <t>Nguyễn Thị</t>
@@ -157,18 +145,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,17 +177,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86571EA6-E2F5-44D1-85B1-47F8112D8ED6}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,12 +514,11 @@
     <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -556,7 +532,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>10</v>
@@ -571,125 +547,108 @@
         <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{02E26573-3700-49D6-937A-154191AA3BBE}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{A7B8AAF0-F277-4C7B-A523-66EC8D98A871}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{08A97626-1187-4AD6-AE18-A08EF734D965}"/>
-  </hyperlinks>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>